<commit_message>
added some styles on ui side
</commit_message>
<xml_diff>
--- a/project/src/assets/Data.xlsx
+++ b/project/src/assets/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Angular_Assignment\project\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945D816C-3C0A-4C94-855A-77BAA2F86E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CEDF15-9085-413C-9882-900500A54CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BCE59C97-D87D-4094-ACE4-A0E381088985}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8964" xr2:uid="{BCE59C97-D87D-4094-ACE4-A0E381088985}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1923,7 +1923,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>